<commit_message>
Refactor: Remove OpenBB/OpenFIGI, switch to manual price ingestion, update docs
</commit_message>
<xml_diff>
--- a/0. Requirements/PortfolioData.xlsx
+++ b/0. Requirements/PortfolioData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PerixMonitor\0. Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FA2ADE-F9A3-4A56-9C5B-D470D3DD81E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10452012-AB70-4069-9437-8011D9DE16CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="980" windowWidth="28800" windowHeight="15460" xr2:uid="{461EA0C3-CC98-4DCD-BC5C-C997A9959903}"/>
+    <workbookView xWindow="720" yWindow="1320" windowWidth="28800" windowHeight="15460" xr2:uid="{461EA0C3-CC98-4DCD-BC5C-C997A9959903}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="71">
   <si>
     <t>Descrizione Titolo</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Operazione</t>
   </si>
   <si>
-    <t>Prezzo Operazione</t>
-  </si>
-  <si>
     <t>Acquisto</t>
   </si>
   <si>
@@ -280,6 +277,12 @@
   </si>
   <si>
     <t>DE000VG2U9L9</t>
+  </si>
+  <si>
+    <t>Prezzo Corrente (EUR)</t>
+  </si>
+  <si>
+    <t>Prezzo Operazione (EUR)</t>
   </si>
 </sst>
 </file>
@@ -384,10 +387,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{840B4B52-5CB9-41B5-89C1-B1D0A0795C06}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -737,10 +738,11 @@
     <col min="5" max="5" width="17.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.54296875" customWidth="1"/>
-    <col min="8" max="8" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -763,654 +765,685 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="C2" s="4">
         <v>23.643999999999998</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="4">
         <v>506.24740000000003</v>
       </c>
-      <c r="F2" s="6">
-        <v>46036</v>
-      </c>
+      <c r="F2" s="7"/>
       <c r="G2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="4">
-        <v>506.24740000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="C3" s="4">
         <v>1739.742</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="4">
         <v>5.8490000000000002</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="F3" s="7"/>
       <c r="G3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="7"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="C4" s="4">
         <v>364.09</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="4">
         <v>18.447199999999999</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="7"/>
       <c r="G4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="C5" s="4">
         <v>150</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="7">
+        <v>11</v>
+      </c>
+      <c r="E5" s="6">
         <v>156</v>
       </c>
-      <c r="F5" s="6">
-        <v>46036</v>
-      </c>
+      <c r="F5" s="7"/>
       <c r="G5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="7">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="C6" s="4">
         <v>110</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="4">
         <v>91.193799999999996</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="F6" s="7"/>
       <c r="G6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="C7" s="4">
         <v>150</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" s="4">
         <v>99.236699999999999</v>
       </c>
-      <c r="F7" s="4"/>
+      <c r="F7" s="7"/>
       <c r="G7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="C8" s="4">
         <v>10</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="4">
         <v>904.20500000000004</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="7"/>
       <c r="G8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="C9" s="4">
         <v>11</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" s="4">
         <v>986.06179999999995</v>
       </c>
-      <c r="F9" s="4"/>
+      <c r="F9" s="7"/>
       <c r="G9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="C10" s="4">
         <v>12000</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" s="4">
         <v>89.122200000000007</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="7"/>
       <c r="G10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="C11" s="4">
         <v>59.204999999999998</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" s="4">
         <v>253.0189</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="F11" s="7"/>
       <c r="G11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="C12" s="4">
         <v>46.465000000000003</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E12" s="4">
         <v>236.52</v>
       </c>
-      <c r="F12" s="4"/>
+      <c r="F12" s="7"/>
       <c r="G12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="C13" s="4">
         <v>151.94900000000001</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13" s="4">
         <v>164.39670000000001</v>
       </c>
-      <c r="F13" s="4"/>
+      <c r="F13" s="7"/>
       <c r="G13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="C14" s="4">
         <v>1058.7619999999999</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14" s="4">
         <v>9.9169999999999998</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="7">
+        <v>45292</v>
+      </c>
       <c r="G14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="H14" s="4">
+        <f>+E14</f>
+        <v>9.9169999999999998</v>
+      </c>
+      <c r="I14" s="4">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="C15" s="4">
         <v>962.96799999999996</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E15" s="4">
         <v>6.2480000000000002</v>
       </c>
-      <c r="F15" s="4"/>
+      <c r="F15" s="7"/>
       <c r="G15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="C16" s="4">
         <v>993.46</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E16" s="4">
         <v>22.583600000000001</v>
       </c>
-      <c r="F16" s="4"/>
+      <c r="F16" s="7"/>
       <c r="G16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="C17" s="4">
         <v>423.15</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E17" s="4">
         <v>22.7121</v>
       </c>
-      <c r="F17" s="4"/>
+      <c r="F17" s="7"/>
       <c r="G17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="C18" s="4">
         <v>70</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E18" s="4">
         <v>100.5106</v>
       </c>
-      <c r="F18" s="4"/>
+      <c r="F18" s="7"/>
       <c r="G18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="C19" s="4">
         <v>33.834000000000003</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E19" s="4">
         <v>227.53</v>
       </c>
-      <c r="F19" s="4"/>
+      <c r="F19" s="7"/>
       <c r="G19" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="C20" s="4">
         <v>78</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E20" s="4">
         <v>105.6832</v>
       </c>
-      <c r="F20" s="4"/>
+      <c r="F20" s="7"/>
       <c r="G20" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="C21" s="4">
         <v>6970.3670000000002</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E21" s="4">
         <v>5.0183999999999997</v>
       </c>
-      <c r="F21" s="4"/>
+      <c r="F21" s="7"/>
       <c r="G21" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="C22" s="4">
         <v>573.66899999999998</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E22" s="4">
         <v>31.342099999999999</v>
       </c>
-      <c r="F22" s="4"/>
+      <c r="F22" s="7"/>
       <c r="G22" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="C23" s="4">
         <v>95.162000000000006</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E23" s="4">
         <v>187.31389999999999</v>
       </c>
-      <c r="F23" s="4"/>
+      <c r="F23" s="7"/>
       <c r="G23" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="C24" s="4">
         <v>132.68199999999999</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E24" s="4">
         <v>133.99940000000001</v>
       </c>
-      <c r="F24" s="4"/>
+      <c r="F24" s="7"/>
       <c r="G24" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="C25" s="4">
         <v>69.063999999999993</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E25" s="4">
         <v>178.98509999999999</v>
       </c>
-      <c r="F25" s="4"/>
+      <c r="F25" s="7"/>
       <c r="G25" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="C26" s="4">
         <v>150</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E26" s="4">
         <v>40.496299999999998</v>
       </c>
-      <c r="F26" s="4"/>
+      <c r="F26" s="7"/>
       <c r="G26" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H26" s="7"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="C27" s="4">
         <v>99.9</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E27" s="4">
         <v>100</v>
       </c>
-      <c r="F27" s="4"/>
+      <c r="F27" s="7"/>
       <c r="G27" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="7"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="C28" s="4">
         <v>110</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E28" s="4">
         <v>39.818899999999999</v>
       </c>
-      <c r="F28" s="4"/>
+      <c r="F28" s="7"/>
       <c r="G28" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="C29" s="4">
         <v>203</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E29" s="4">
         <v>35.979500000000002</v>
       </c>
-      <c r="F29" s="4"/>
+      <c r="F29" s="7"/>
       <c r="G29" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H29" s="7"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="C30" s="4">
         <v>120</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E30" s="4">
         <v>97.274799999999999</v>
       </c>
-      <c r="F30" s="4"/>
+      <c r="F30" s="7"/>
       <c r="G30" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H30" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
feat(dashboard): add asset filtering and time window slider, refine ingestion logic
</commit_message>
<xml_diff>
--- a/0. Requirements/PortfolioData.xlsx
+++ b/0. Requirements/PortfolioData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PerixMonitor\0. Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10452012-AB70-4069-9437-8011D9DE16CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB17931-5D95-49E1-97DB-EB4945324681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="1320" windowWidth="28800" windowHeight="15460" xr2:uid="{461EA0C3-CC98-4DCD-BC5C-C997A9959903}"/>
+    <workbookView xWindow="-110" yWindow="490" windowWidth="38620" windowHeight="21220" xr2:uid="{461EA0C3-CC98-4DCD-BC5C-C997A9959903}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="70">
   <si>
     <t>Descrizione Titolo</t>
   </si>
@@ -93,196 +93,193 @@
     <t>Operazione</t>
   </si>
   <si>
+    <t>ACMB IL HEALTH C EUR</t>
+  </si>
+  <si>
+    <t>LU0251853072</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>ANIMA TRICOL A</t>
+  </si>
+  <si>
+    <t>IT0005186082</t>
+  </si>
+  <si>
+    <t>BGF WLD ENERG E2 EUR</t>
+  </si>
+  <si>
+    <t>LU0171304552</t>
+  </si>
+  <si>
+    <t>BPA CC E28</t>
+  </si>
+  <si>
+    <t>NLBNPIT2OWW8</t>
+  </si>
+  <si>
+    <t>BSKT/BNPI 28</t>
+  </si>
+  <si>
+    <t>XS3124062178</t>
+  </si>
+  <si>
+    <t>BSKT/BNPI 28 0.85%</t>
+  </si>
+  <si>
+    <t>XS3174995152</t>
+  </si>
+  <si>
+    <t>BSKT/LEON 27</t>
+  </si>
+  <si>
+    <t>CH1290280945</t>
+  </si>
+  <si>
+    <t>BSKT/LEON 29</t>
+  </si>
+  <si>
+    <t>CH1467578527</t>
+  </si>
+  <si>
+    <t>BTP SETTEMB 27 0.95%</t>
+  </si>
+  <si>
+    <t>IT0005416570</t>
+  </si>
+  <si>
+    <t>CAN BD GL HY CC  EUR</t>
+  </si>
+  <si>
+    <t>LU0170291933</t>
+  </si>
+  <si>
+    <t>D INV I C SECT LCC</t>
+  </si>
+  <si>
+    <t>LU1278917452</t>
+  </si>
+  <si>
+    <t>DWS CONC KALDEM  EUR</t>
+  </si>
+  <si>
+    <t>LU0599946893</t>
+  </si>
+  <si>
+    <t>EURIZON OB E HY</t>
+  </si>
+  <si>
+    <t>IT0001280541</t>
+  </si>
+  <si>
+    <t>EURIZON OB EC</t>
+  </si>
+  <si>
+    <t>IT0003459473</t>
+  </si>
+  <si>
+    <t>FID CHINA CONS E EUR</t>
+  </si>
+  <si>
+    <t>LU0766124126</t>
+  </si>
+  <si>
+    <t>FID GLO DEMO E EUH A</t>
+  </si>
+  <si>
+    <t>LU0528228157</t>
+  </si>
+  <si>
+    <t>ISHS MSCI WORLD EUR</t>
+  </si>
+  <si>
+    <t>IE00B4L5Y983</t>
+  </si>
+  <si>
+    <t>JPMIF GL DIV AC  EUR</t>
+  </si>
+  <si>
+    <t>LU0329202252</t>
+  </si>
+  <si>
+    <t>LIF EM 1-3YIBGB  EUR</t>
+  </si>
+  <si>
+    <t>LU1598691050</t>
+  </si>
+  <si>
+    <t>MB MFS PRUD CAP K AC</t>
+  </si>
+  <si>
+    <t>IT0005444754</t>
+  </si>
+  <si>
+    <t>MSI EU C B D H"A"ACC</t>
+  </si>
+  <si>
+    <t>LU1832969650</t>
+  </si>
+  <si>
+    <t>MSIF GL BRDS AC</t>
+  </si>
+  <si>
+    <t>LU0119620416</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>N1 EU CR CRED BP EUR</t>
+  </si>
+  <si>
+    <t>LU0733673288</t>
+  </si>
+  <si>
+    <t>N1 EUR BANK D BP EUR</t>
+  </si>
+  <si>
+    <t>LU0772944145</t>
+  </si>
+  <si>
+    <t>TC MOR HIGH DIV  EUR</t>
+  </si>
+  <si>
+    <t>NL0011683594</t>
+  </si>
+  <si>
+    <t>U ACCESS SICAV - EUR</t>
+  </si>
+  <si>
+    <t>LU2695671391</t>
+  </si>
+  <si>
+    <t>VAN VEC SE USD-A EUR</t>
+  </si>
+  <si>
+    <t>IE00BMC38736</t>
+  </si>
+  <si>
+    <t>VANECK DEFENSE EUR</t>
+  </si>
+  <si>
+    <t>IE000YYE6WK5</t>
+  </si>
+  <si>
+    <t>VON EXPE27</t>
+  </si>
+  <si>
+    <t>DE000VG2U9L9</t>
+  </si>
+  <si>
+    <t>Prezzo Corrente (EUR)</t>
+  </si>
+  <si>
+    <t>Prezzo Operazione (EUR)</t>
+  </si>
+  <si>
     <t>Acquisto</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>ACMB IL HEALTH C EUR</t>
-  </si>
-  <si>
-    <t>LU0251853072</t>
-  </si>
-  <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>ANIMA TRICOL A</t>
-  </si>
-  <si>
-    <t>IT0005186082</t>
-  </si>
-  <si>
-    <t>BGF WLD ENERG E2 EUR</t>
-  </si>
-  <si>
-    <t>LU0171304552</t>
-  </si>
-  <si>
-    <t>BPA CC E28</t>
-  </si>
-  <si>
-    <t>NLBNPIT2OWW8</t>
-  </si>
-  <si>
-    <t>BSKT/BNPI 28</t>
-  </si>
-  <si>
-    <t>XS3124062178</t>
-  </si>
-  <si>
-    <t>BSKT/BNPI 28 0.85%</t>
-  </si>
-  <si>
-    <t>XS3174995152</t>
-  </si>
-  <si>
-    <t>BSKT/LEON 27</t>
-  </si>
-  <si>
-    <t>CH1290280945</t>
-  </si>
-  <si>
-    <t>BSKT/LEON 29</t>
-  </si>
-  <si>
-    <t>CH1467578527</t>
-  </si>
-  <si>
-    <t>BTP SETTEMB 27 0.95%</t>
-  </si>
-  <si>
-    <t>IT0005416570</t>
-  </si>
-  <si>
-    <t>CAN BD GL HY CC  EUR</t>
-  </si>
-  <si>
-    <t>LU0170291933</t>
-  </si>
-  <si>
-    <t>D INV I C SECT LCC</t>
-  </si>
-  <si>
-    <t>LU1278917452</t>
-  </si>
-  <si>
-    <t>DWS CONC KALDEM  EUR</t>
-  </si>
-  <si>
-    <t>LU0599946893</t>
-  </si>
-  <si>
-    <t>EURIZON OB E HY</t>
-  </si>
-  <si>
-    <t>IT0001280541</t>
-  </si>
-  <si>
-    <t>EURIZON OB EC</t>
-  </si>
-  <si>
-    <t>IT0003459473</t>
-  </si>
-  <si>
-    <t>FID CHINA CONS E EUR</t>
-  </si>
-  <si>
-    <t>LU0766124126</t>
-  </si>
-  <si>
-    <t>FID GLO DEMO E EUH A</t>
-  </si>
-  <si>
-    <t>LU0528228157</t>
-  </si>
-  <si>
-    <t>ISHS MSCI WORLD EUR</t>
-  </si>
-  <si>
-    <t>IE00B4L5Y983</t>
-  </si>
-  <si>
-    <t>JPMIF GL DIV AC  EUR</t>
-  </si>
-  <si>
-    <t>LU0329202252</t>
-  </si>
-  <si>
-    <t>LIF EM 1-3YIBGB  EUR</t>
-  </si>
-  <si>
-    <t>LU1598691050</t>
-  </si>
-  <si>
-    <t>MB MFS PRUD CAP K AC</t>
-  </si>
-  <si>
-    <t>IT0005444754</t>
-  </si>
-  <si>
-    <t>MSI EU C B D H"A"ACC</t>
-  </si>
-  <si>
-    <t>LU1832969650</t>
-  </si>
-  <si>
-    <t>MSIF GL BRDS AC</t>
-  </si>
-  <si>
-    <t>LU0119620416</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>N1 EU CR CRED BP EUR</t>
-  </si>
-  <si>
-    <t>LU0733673288</t>
-  </si>
-  <si>
-    <t>N1 EUR BANK D BP EUR</t>
-  </si>
-  <si>
-    <t>LU0772944145</t>
-  </si>
-  <si>
-    <t>TC MOR HIGH DIV  EUR</t>
-  </si>
-  <si>
-    <t>NL0011683594</t>
-  </si>
-  <si>
-    <t>U ACCESS SICAV - EUR</t>
-  </si>
-  <si>
-    <t>LU2695671391</t>
-  </si>
-  <si>
-    <t>VAN VEC SE USD-A EUR</t>
-  </si>
-  <si>
-    <t>IE00BMC38736</t>
-  </si>
-  <si>
-    <t>VANECK DEFENSE EUR</t>
-  </si>
-  <si>
-    <t>IE000YYE6WK5</t>
-  </si>
-  <si>
-    <t>VON EXPE27</t>
-  </si>
-  <si>
-    <t>DE000VG2U9L9</t>
-  </si>
-  <si>
-    <t>Prezzo Corrente (EUR)</t>
-  </si>
-  <si>
-    <t>Prezzo Operazione (EUR)</t>
   </si>
 </sst>
 </file>
@@ -726,7 +723,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -765,689 +762,857 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" s="4">
         <v>23.643999999999998</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E2" s="4">
         <v>506.24740000000003</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="7">
+        <v>46036</v>
+      </c>
       <c r="G2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+        <v>69</v>
+      </c>
+      <c r="H2" s="4">
+        <v>515.6</v>
+      </c>
+      <c r="I2" s="4">
+        <v>515.6</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" s="4">
         <v>1739.742</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E3" s="4">
         <v>5.8490000000000002</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="7">
+        <v>46036</v>
+      </c>
       <c r="G3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H3" s="6">
+        <v>6.8029999999999999</v>
+      </c>
+      <c r="I3" s="6">
+        <v>6.8029999999999999</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="4">
         <v>364.09</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" s="4">
         <v>18.447199999999999</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="7">
+        <v>46036</v>
+      </c>
       <c r="G4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H4" s="6">
+        <v>21.02</v>
+      </c>
+      <c r="I4" s="6">
+        <v>21.02</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4">
         <v>150</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" s="6">
-        <v>156</v>
-      </c>
-      <c r="F5" s="7"/>
+        <v>100.3967</v>
+      </c>
+      <c r="F5" s="7">
+        <v>46036</v>
+      </c>
       <c r="G5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H5" s="6">
+        <v>103.04</v>
+      </c>
+      <c r="I5" s="6">
+        <v>103.04</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" s="4">
         <v>110</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E6" s="4">
         <v>91.193799999999996</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="7">
+        <v>46036</v>
+      </c>
       <c r="G6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H6" s="6">
+        <v>96.85</v>
+      </c>
+      <c r="I6" s="6">
+        <v>96.85</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="4">
         <v>150</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E7" s="4">
         <v>99.236699999999999</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="7">
+        <v>46036</v>
+      </c>
       <c r="G7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H7" s="6">
+        <v>97.53</v>
+      </c>
+      <c r="I7" s="6">
+        <v>97.53</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" s="4">
         <v>10</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E8" s="4">
         <v>904.20500000000004</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="7">
+        <v>46036</v>
+      </c>
       <c r="G8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H8" s="6">
+        <v>677.76</v>
+      </c>
+      <c r="I8" s="6">
+        <v>677.76</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" s="4">
         <v>11</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E9" s="4">
         <v>986.06179999999995</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="7">
+        <v>46036</v>
+      </c>
       <c r="G9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H9" s="6">
+        <v>679.32</v>
+      </c>
+      <c r="I9" s="6">
+        <v>679.32</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="4">
-        <v>12000</v>
+        <f>12000*0.01</f>
+        <v>120</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E10" s="4">
         <v>89.122200000000007</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="7">
+        <v>46036</v>
+      </c>
       <c r="G10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H10" s="6">
+        <v>98.12</v>
+      </c>
+      <c r="I10" s="6">
+        <v>98.12</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11" s="4">
         <v>59.204999999999998</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E11" s="4">
         <v>253.0189</v>
       </c>
-      <c r="F11" s="7"/>
+      <c r="F11" s="7">
+        <v>46036</v>
+      </c>
       <c r="G11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H11" s="6">
+        <v>291.01</v>
+      </c>
+      <c r="I11" s="6">
+        <v>291.01</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C12" s="4">
         <v>46.465000000000003</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E12" s="4">
         <v>236.52</v>
       </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="7">
+        <v>46036</v>
+      </c>
       <c r="G12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H12" s="6">
+        <v>259.68</v>
+      </c>
+      <c r="I12" s="6">
+        <v>259.68</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C13" s="4">
         <v>151.94900000000001</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E13" s="4">
         <v>164.39670000000001</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="7">
+        <v>46036</v>
+      </c>
       <c r="G13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H13" s="6">
+        <v>186.04</v>
+      </c>
+      <c r="I13" s="6">
+        <v>186.04</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C14" s="4">
         <v>1058.7619999999999</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E14" s="4">
         <v>9.9169999999999998</v>
       </c>
       <c r="F14" s="7">
-        <v>45292</v>
+        <v>46036</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="H14" s="4">
-        <f>+E14</f>
-        <v>9.9169999999999998</v>
+        <v>12.096</v>
       </c>
       <c r="I14" s="4">
-        <v>10.5</v>
+        <v>12.096</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="4">
         <v>962.96799999999996</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E15" s="4">
         <v>6.2480000000000002</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="7">
+        <v>46036</v>
+      </c>
       <c r="G15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H15" s="6">
+        <v>7.2519999999999998</v>
+      </c>
+      <c r="I15" s="6">
+        <v>7.2519999999999998</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C16" s="4">
         <v>993.46</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E16" s="4">
         <v>22.583600000000001</v>
       </c>
-      <c r="F16" s="7"/>
+      <c r="F16" s="7">
+        <v>46036</v>
+      </c>
       <c r="G16" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H16" s="6">
+        <v>18</v>
+      </c>
+      <c r="I16" s="6">
+        <v>18</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" s="4">
         <v>423.15</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E17" s="4">
         <v>22.7121</v>
       </c>
-      <c r="F17" s="7"/>
+      <c r="F17" s="7">
+        <v>46036</v>
+      </c>
       <c r="G17" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H17" s="6">
+        <v>28.25</v>
+      </c>
+      <c r="I17" s="6">
+        <v>28.25</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C18" s="4">
         <v>70</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E18" s="4">
         <v>100.5106</v>
       </c>
-      <c r="F18" s="7"/>
+      <c r="F18" s="7">
+        <v>46036</v>
+      </c>
       <c r="G18" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H18" s="6">
+        <v>114.95</v>
+      </c>
+      <c r="I18" s="6">
+        <v>114.95</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C19" s="4">
         <v>33.834000000000003</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E19" s="4">
         <v>227.53</v>
       </c>
-      <c r="F19" s="7"/>
+      <c r="F19" s="7">
+        <v>46036</v>
+      </c>
       <c r="G19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H19" s="6">
+        <v>305.91000000000003</v>
+      </c>
+      <c r="I19" s="6">
+        <v>305.91000000000003</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C20" s="4">
         <v>78</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E20" s="4">
         <v>105.6832</v>
       </c>
-      <c r="F20" s="7"/>
+      <c r="F20" s="7">
+        <v>46036</v>
+      </c>
       <c r="G20" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H20" s="6">
+        <v>104.66</v>
+      </c>
+      <c r="I20" s="6">
+        <v>104.66</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C21" s="4">
         <v>6970.3670000000002</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E21" s="4">
         <v>5.0183999999999997</v>
       </c>
-      <c r="F21" s="7"/>
+      <c r="F21" s="7">
+        <v>46036</v>
+      </c>
       <c r="G21" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H21" s="6">
+        <v>5.9420000000000002</v>
+      </c>
+      <c r="I21" s="6">
+        <v>5.9420000000000002</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C22" s="4">
         <v>573.66899999999998</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E22" s="4">
         <v>31.342099999999999</v>
       </c>
-      <c r="F22" s="7"/>
+      <c r="F22" s="7">
+        <v>46036</v>
+      </c>
       <c r="G22" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H22" s="6">
+        <v>35.07</v>
+      </c>
+      <c r="I22" s="6">
+        <v>35.07</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C23" s="4">
         <v>95.162000000000006</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E23" s="4">
         <v>187.31389999999999</v>
       </c>
-      <c r="F23" s="7"/>
+      <c r="F23" s="7">
+        <v>46036</v>
+      </c>
       <c r="G23" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H23" s="6">
+        <v>191.92429999999999</v>
+      </c>
+      <c r="I23" s="6">
+        <v>191.92429999999999</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C24" s="4">
         <v>132.68199999999999</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E24" s="4">
         <v>133.99940000000001</v>
       </c>
-      <c r="F24" s="7"/>
+      <c r="F24" s="7">
+        <v>46036</v>
+      </c>
       <c r="G24" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H24" s="6">
+        <v>147.6463</v>
+      </c>
+      <c r="I24" s="6">
+        <v>147.6463</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C25" s="4">
         <v>69.063999999999993</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E25" s="4">
         <v>178.98509999999999</v>
       </c>
-      <c r="F25" s="7"/>
+      <c r="F25" s="7">
+        <v>46036</v>
+      </c>
       <c r="G25" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H25" s="6">
+        <v>210.4076</v>
+      </c>
+      <c r="I25" s="6">
+        <v>210.4076</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C26" s="4">
         <v>150</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E26" s="4">
         <v>40.496299999999998</v>
       </c>
-      <c r="F26" s="7"/>
+      <c r="F26" s="7">
+        <v>46036</v>
+      </c>
       <c r="G26" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H26" s="6">
+        <v>49.12</v>
+      </c>
+      <c r="I26" s="6">
+        <v>49.12</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C27" s="4">
         <v>99.9</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E27" s="4">
         <v>100</v>
       </c>
-      <c r="F27" s="7"/>
+      <c r="F27" s="7">
+        <v>46036</v>
+      </c>
       <c r="G27" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H27" s="6">
+        <v>105.74</v>
+      </c>
+      <c r="I27" s="6">
+        <v>105.74</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C28" s="4">
         <v>110</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E28" s="4">
         <v>39.818899999999999</v>
       </c>
-      <c r="F28" s="7"/>
+      <c r="F28" s="7">
+        <v>46036</v>
+      </c>
       <c r="G28" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H28" s="6">
+        <v>60.58</v>
+      </c>
+      <c r="I28" s="6">
+        <v>60.58</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C29" s="4">
         <v>203</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E29" s="4">
         <v>35.979500000000002</v>
       </c>
-      <c r="F29" s="7"/>
+      <c r="F29" s="7">
+        <v>46036</v>
+      </c>
       <c r="G29" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H29" s="6">
+        <v>63.3</v>
+      </c>
+      <c r="I29" s="6">
+        <v>63.3</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C30" s="4">
         <v>120</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E30" s="4">
         <v>97.274799999999999</v>
       </c>
-      <c r="F30" s="7"/>
+      <c r="F30" s="7">
+        <v>46036</v>
+      </c>
       <c r="G30" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="H30" s="6">
+        <v>100.44</v>
+      </c>
+      <c r="I30" s="6">
+        <v>100.44</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G30" xr:uid="{8B74CA58-03E8-45C3-8C73-E3434A7DC53B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G30" xr:uid="{786B1B08-543B-41BE-8266-499A04655516}">
       <formula1>"Acquisto,Vendita,-"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>